<commit_message>
get oilcane biorefinery ready for users
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-2_agile.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-2_agile.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\Code\bioindustrial-park\BioSTEAM 2.x.x\biorefineries\oilcane\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB00CBD6-E409-4571-B5DA-D1CFD06F5C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>Element</t>
   </si>
@@ -94,6 +88,9 @@
     <t>Stream-pure glycerine</t>
   </si>
   <si>
+    <t>Saccharification</t>
+  </si>
+  <si>
     <t>cellulase</t>
   </si>
   <si>
@@ -109,6 +106,18 @@
     <t>Cofermentation</t>
   </si>
   <si>
+    <t>oilcane</t>
+  </si>
+  <si>
+    <t>oilsorghum</t>
+  </si>
+  <si>
+    <t>Oil retention [%]</t>
+  </si>
+  <si>
+    <t>Bagasse oil extraction efficiency [%]</t>
+  </si>
+  <si>
     <t>Capacity [ton/hr]</t>
   </si>
   <si>
@@ -130,7 +139,7 @@
     <t>Price [USD/kg]</t>
   </si>
   <si>
-    <t>Tau</t>
+    <t>Reaction time [hr]</t>
   </si>
   <si>
     <t>Cellulase loading [wt. % cellulose]</t>
@@ -163,18 +172,9 @@
     <t>Productivity [g/L]</t>
   </si>
   <si>
-    <t>Bagasse oil extraction efficiency [%]</t>
-  </si>
-  <si>
-    <t>oilcane</t>
-  </si>
-  <si>
     <t>Cane  PL content [% oil]</t>
   </si>
   <si>
-    <t>oilsorghum</t>
-  </si>
-  <si>
     <t>Sorghum  PL content [% oil]</t>
   </si>
   <si>
@@ -191,16 +191,13 @@
   </si>
   <si>
     <t>TAG to  FFA conversion [% oil]</t>
-  </si>
-  <si>
-    <t>Oil retention [%]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,11 +249,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -266,14 +260,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -320,7 +306,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -352,27 +338,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,24 +372,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -597,37 +547,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -674,7 +622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,865 +630,865 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:16">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C4">
-        <v>-2.1937664653506581E-2</v>
+        <v>-0.02178606327144253</v>
       </c>
       <c r="E4">
-        <v>1.017420424696817E-3</v>
+        <v>0.001017420424696817</v>
       </c>
       <c r="F4">
-        <v>6.2119659686195837E-3</v>
+        <v>0.008873367245824569</v>
       </c>
       <c r="G4">
-        <v>9.7839535445031559E-3</v>
+        <v>0.006631759320898819</v>
       </c>
       <c r="H4">
-        <v>2.181278535251141E-2</v>
+        <v>0.02163572544142901</v>
       </c>
       <c r="I4">
-        <v>1.9732750005309999E-2</v>
+        <v>0.01973405570136223</v>
       </c>
       <c r="J4">
-        <v>4.6664576650420203E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+        <v>0.004047648023928821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C5">
-        <v>6.2114068404562732E-3</v>
+        <v>0.006244974681798986</v>
       </c>
       <c r="E5">
-        <v>-2.431366369254654E-2</v>
+        <v>-0.02431366369254654</v>
       </c>
       <c r="F5">
-        <v>7.2389608369982988E-3</v>
+        <v>-0.004555328027679798</v>
       </c>
       <c r="G5">
-        <v>-1.2782265045500949E-2</v>
+        <v>-0.005027616043633179</v>
       </c>
       <c r="H5">
-        <v>2.045212651408506E-2</v>
+        <v>0.02058372072734883</v>
       </c>
       <c r="I5">
-        <v>2.1703847524153899E-2</v>
+        <v>0.02170356662814266</v>
       </c>
       <c r="J5">
-        <v>6.0769064753894673E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
+        <v>0.005235899113226982</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C6">
-        <v>0.14010158355606331</v>
+        <v>0.1461728851109154</v>
       </c>
       <c r="E6">
-        <v>4.4739630589585208E-4</v>
+        <v>0.0004473963058958521</v>
       </c>
       <c r="F6">
-        <v>-0.19129478041647219</v>
+        <v>-0.1620529528657556</v>
       </c>
       <c r="G6">
-        <v>0.2015238379861623</v>
+        <v>0.2110682397058556</v>
       </c>
       <c r="H6">
-        <v>0.97684953436998123</v>
+        <v>0.9792522406100895</v>
       </c>
       <c r="I6">
-        <v>0.9749380372055213</v>
+        <v>0.9749379199895165</v>
       </c>
       <c r="J6">
-        <v>-0.43723373711148522</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>-0.4358742691555516</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C7">
-        <v>0.94871165801246604</v>
+        <v>0.9451639506065579</v>
       </c>
       <c r="E7">
-        <v>-1.6837912225516491E-2</v>
+        <v>-0.01683791222551649</v>
       </c>
       <c r="F7">
-        <v>3.4532208090815773E-2</v>
+        <v>0.02523746121209629</v>
       </c>
       <c r="G7">
-        <v>-2.1215653709267181E-2</v>
+        <v>-0.01642449027200107</v>
       </c>
       <c r="H7">
-        <v>2.5132973805318948E-4</v>
+        <v>-7.207488288299531E-05</v>
       </c>
       <c r="I7">
-        <v>9.388744695549788E-4</v>
+        <v>0.0009378093495123737</v>
       </c>
       <c r="J7">
-        <v>1.3484506685827071E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.0147719677808594</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C8">
-        <v>2.161780684871227E-2</v>
+        <v>0.02159808854392354</v>
       </c>
       <c r="E8">
-        <v>2.9479245339169811E-3</v>
+        <v>0.002947924533916981</v>
       </c>
       <c r="F8">
-        <v>-1.799247507815692E-3</v>
+        <v>-0.001435201649397467</v>
       </c>
       <c r="G8">
-        <v>1.1427191264899741E-2</v>
+        <v>0.009023845602815066</v>
       </c>
       <c r="H8">
-        <v>1.351200553248022E-2</v>
+        <v>0.01358505807940232</v>
       </c>
       <c r="I8">
-        <v>1.7057258794290351E-2</v>
+        <v>0.01705835175433407</v>
       </c>
       <c r="J8">
-        <v>2.8316089171379968E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.002669921342769697</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C9">
-        <v>-3.7486534619461378E-3</v>
+        <v>-0.004956136038245441</v>
       </c>
       <c r="E9">
-        <v>2.7202657088106277E-4</v>
+        <v>0.0002720265708810628</v>
       </c>
       <c r="F9">
-        <v>-2.342008749204079E-3</v>
+        <v>-0.01249334876587546</v>
       </c>
       <c r="G9">
-        <v>-1.2304510242468101E-2</v>
+        <v>-0.01048073791044328</v>
       </c>
       <c r="H9">
-        <v>-1.7228010065120401E-2</v>
+        <v>-0.01716079201443168</v>
       </c>
       <c r="I9">
-        <v>-1.634195143767805E-2</v>
+        <v>-0.01634075134163005</v>
       </c>
       <c r="J9">
-        <v>-1.162517198491011E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+        <v>-0.01059737405566386</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C10">
-        <v>9.393118935724757E-3</v>
+        <v>0.009240065457602616</v>
       </c>
       <c r="E10">
-        <v>-1.8701300428052011E-2</v>
+        <v>-0.01870130042805201</v>
       </c>
       <c r="F10">
-        <v>1.4897670811083759E-2</v>
+        <v>0.007718071258129879</v>
       </c>
       <c r="G10">
-        <v>-9.3574927185277323E-3</v>
+        <v>-0.008054564377493634</v>
       </c>
       <c r="H10">
-        <v>1.282621692904868E-2</v>
+        <v>0.01297155671086227</v>
       </c>
       <c r="I10">
-        <v>1.5170284158811361E-2</v>
+        <v>0.01517033091081323</v>
       </c>
       <c r="J10">
-        <v>8.2744014302954371E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+        <v>0.008558100883058488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C11">
-        <v>0.1147579658703186</v>
+        <v>0.1179754348950174</v>
       </c>
       <c r="E11">
-        <v>2.049043195561728E-2</v>
+        <v>0.02049043195561728</v>
       </c>
       <c r="F11">
-        <v>-2.2503474387140711E-2</v>
+        <v>-0.002575221489738423</v>
       </c>
       <c r="G11">
-        <v>1.9211651200486499E-2</v>
+        <v>0.01966852721956816</v>
       </c>
       <c r="H11">
-        <v>4.1720480388819214E-3</v>
+        <v>0.004754827486193099</v>
       </c>
       <c r="I11">
-        <v>0.22390094585203779</v>
+        <v>0.2239014582040583</v>
       </c>
       <c r="J11">
-        <v>-5.4655109140972552E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+        <v>-0.005330211965139834</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C12">
-        <v>-0.1865834734793389</v>
+        <v>-0.1944687593307503</v>
       </c>
       <c r="E12">
-        <v>1.274416966176679E-2</v>
+        <v>0.01274416966176679</v>
       </c>
       <c r="F12">
-        <v>-1.43719358610077E-2</v>
+        <v>-0.02403284048275976</v>
       </c>
       <c r="G12">
-        <v>2.474078181510278E-2</v>
+        <v>0.02023854292754859</v>
       </c>
       <c r="H12">
-        <v>1.404875921795037E-2</v>
+        <v>0.01420801784832071</v>
       </c>
       <c r="I12">
-        <v>1.7457324410292969E-2</v>
+        <v>0.0174572575942903</v>
       </c>
       <c r="J12">
-        <v>-1.6682156610107451E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <v>-0.01610976849236207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>1.9689991219599651E-2</v>
+        <v>0.01982688290507531</v>
       </c>
       <c r="E13">
-        <v>-1.8565329574613178E-2</v>
+        <v>-0.01856532957461318</v>
       </c>
       <c r="F13">
-        <v>6.9675929489250782E-3</v>
+        <v>0.01095787481283199</v>
       </c>
       <c r="G13">
-        <v>-8.3272087113071963E-3</v>
+        <v>-0.01189840659251182</v>
       </c>
       <c r="H13">
-        <v>-2.9185383567415339E-3</v>
+        <v>-0.002921853140874125</v>
       </c>
       <c r="I13">
-        <v>-4.9047487721899496E-3</v>
+        <v>-0.004904482468179298</v>
       </c>
       <c r="J13">
-        <v>7.9624237853895465E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.00833147847365638</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C14">
-        <v>2.0345980653839221E-3</v>
+        <v>0.001805170728206829</v>
       </c>
       <c r="E14">
-        <v>-7.0090912243636469E-3</v>
+        <v>-0.007009091224363647</v>
       </c>
       <c r="F14">
-        <v>-5.8984297357941159E-3</v>
+        <v>0.00378156849679851</v>
       </c>
       <c r="G14">
-        <v>2.7648709168838141E-3</v>
+        <v>0.002995960697059417</v>
       </c>
       <c r="H14">
-        <v>-2.824010128960404E-3</v>
+        <v>-0.002975146103005844</v>
       </c>
       <c r="I14">
-        <v>-8.0747009629880372E-3</v>
+        <v>-0.008074795522991819</v>
       </c>
       <c r="J14">
-        <v>-5.0441897446680409E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>-0.005216447544419975</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C15">
-        <v>-2.1924503244980131E-2</v>
+        <v>-0.0222898449875938</v>
       </c>
       <c r="E15">
-        <v>4.6681906507276246E-3</v>
+        <v>0.004668190650727625</v>
       </c>
       <c r="F15">
-        <v>-9.3344547263127815E-3</v>
+        <v>-0.01032902611266237</v>
       </c>
       <c r="G15">
-        <v>1.1736110110634711E-2</v>
+        <v>0.01050458869304279</v>
       </c>
       <c r="H15">
-        <v>2.3440881577635259E-2</v>
+        <v>0.02241249468849978</v>
       </c>
       <c r="I15">
-        <v>-7.9171167646846698E-3</v>
+        <v>-0.007917184444687376</v>
       </c>
       <c r="J15">
-        <v>8.467293086274981E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>0.009819926855409125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C16">
-        <v>-6.0777597727103887E-2</v>
+        <v>-0.06064486034579441</v>
       </c>
       <c r="E16">
-        <v>9.4010464240418552E-3</v>
+        <v>0.009401046424041855</v>
       </c>
       <c r="F16">
-        <v>-7.3492873733884446E-3</v>
+        <v>-0.002272743482321257</v>
       </c>
       <c r="G16">
-        <v>9.1066295981990682E-3</v>
+        <v>0.007767363540307167</v>
       </c>
       <c r="H16">
-        <v>5.1889673435586928E-3</v>
+        <v>0.005459343194373727</v>
       </c>
       <c r="I16">
-        <v>7.4319407132776268E-3</v>
+        <v>0.007432342089293682</v>
       </c>
       <c r="J16">
-        <v>-1.4712025568607071E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+        <v>-0.0008136725137576451</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C17">
-        <v>2.2373961534958458E-3</v>
+        <v>0.002148286165931446</v>
       </c>
       <c r="E17">
-        <v>-2.742909901716396E-3</v>
+        <v>-0.002742909901716396</v>
       </c>
       <c r="F17">
-        <v>5.1265350768776169E-3</v>
+        <v>0.005157937455579056</v>
       </c>
       <c r="G17">
-        <v>1.0608808760365939E-2</v>
+        <v>0.01174648469745057</v>
       </c>
       <c r="H17">
-        <v>8.4889899395595957E-3</v>
+        <v>0.008542001717680067</v>
       </c>
       <c r="I17">
-        <v>6.1111490444459614E-3</v>
+        <v>0.006111340564453622</v>
       </c>
       <c r="J17">
-        <v>-2.4361433327783769E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-0.002971988331301852</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C18">
-        <v>-3.4561163174446519E-2</v>
+        <v>-0.03450804550832182</v>
       </c>
       <c r="E18">
-        <v>-8.6810933392437329E-3</v>
+        <v>-0.008681093339243733</v>
       </c>
       <c r="F18">
-        <v>4.3309629827162233E-3</v>
+        <v>0.002489322178644055</v>
       </c>
       <c r="G18">
-        <v>7.679919234553979E-3</v>
+        <v>0.007345519945247731</v>
       </c>
       <c r="H18">
-        <v>0.19742360095294401</v>
+        <v>0.189830026377201</v>
       </c>
       <c r="I18">
-        <v>-1.069800042792002E-4</v>
+        <v>-0.0001072122282884891</v>
       </c>
       <c r="J18">
-        <v>2.86134837436826E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>0.001449378828131829</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C19">
-        <v>2.2309267900370709E-2</v>
+        <v>0.02341113184844527</v>
       </c>
       <c r="E19">
-        <v>0.27720640257625612</v>
+        <v>0.2772064025762561</v>
       </c>
       <c r="F19">
-        <v>-0.2582485821188133</v>
+        <v>-0.2453006894465198</v>
       </c>
       <c r="G19">
-        <v>0.34277396535212717</v>
+        <v>0.3549211106169068</v>
       </c>
       <c r="H19">
-        <v>6.8723431548937258E-3</v>
+        <v>0.007507661580306462</v>
       </c>
       <c r="I19">
-        <v>2.1955646318225848E-3</v>
+        <v>0.002195439735817589</v>
       </c>
       <c r="J19">
-        <v>1.6408403238782829E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
+        <v>0.01410233957707786</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C20">
-        <v>-3.9134391965375668E-4</v>
+        <v>-0.0004284536811381472</v>
       </c>
       <c r="E20">
-        <v>0.14953456006138241</v>
+        <v>0.1495345600613824</v>
       </c>
       <c r="F20">
-        <v>-0.1685975315718192</v>
+        <v>-0.1625626329150576</v>
       </c>
       <c r="G20">
-        <v>0.10785747091145199</v>
+        <v>0.1105346451586075</v>
       </c>
       <c r="H20">
-        <v>-3.9858374650334982E-2</v>
+        <v>-0.03439347900773915</v>
       </c>
       <c r="I20">
-        <v>-2.348462397938495E-3</v>
+        <v>-0.002349029949961198</v>
       </c>
       <c r="J20">
-        <v>-0.38711121895801692</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
+        <v>-0.3898497506860864</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C21">
-        <v>2.5568493182739722E-3</v>
+        <v>0.004155616294224652</v>
       </c>
       <c r="E21">
-        <v>0.32673465735738622</v>
+        <v>0.3267346573573862</v>
       </c>
       <c r="F21">
-        <v>-0.20779514165000221</v>
+        <v>-0.1569255335297797</v>
       </c>
       <c r="G21">
-        <v>0.29682799509343483</v>
+        <v>0.2924377355521244</v>
       </c>
       <c r="H21">
-        <v>3.8814068752562741E-3</v>
+        <v>0.003907332924293317</v>
       </c>
       <c r="I21">
-        <v>3.8114983284599328E-3</v>
+        <v>0.003810244472409778</v>
       </c>
       <c r="J21">
-        <v>7.2475808278179227E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
+        <v>0.00822127075708408</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C22">
-        <v>-2.211183822847353E-2</v>
+        <v>-0.02241461667258467</v>
       </c>
       <c r="E22">
-        <v>4.7186308767452343E-3</v>
+        <v>0.004718630876745234</v>
       </c>
       <c r="F22">
-        <v>-2.258434465988398E-2</v>
+        <v>-0.03191199802129083</v>
       </c>
       <c r="G22">
-        <v>-4.6435708305573066E-3</v>
+        <v>0.005389167689688764</v>
       </c>
       <c r="H22">
-        <v>-1.402084731283389E-2</v>
+        <v>-0.01297766067910643</v>
       </c>
       <c r="I22">
-        <v>-1.083848654553946E-2</v>
+        <v>-0.01083829809753192</v>
       </c>
       <c r="J22">
-        <v>-0.18981205558014511</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>-0.1898850109499493</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C23">
-        <v>5.1756003798240142E-2</v>
+        <v>0.0538197277847891</v>
       </c>
       <c r="E23">
         <v>0.5407430554857221</v>
       </c>
       <c r="F23">
-        <v>-0.20536295230505111</v>
+        <v>-0.1524428430707618</v>
       </c>
       <c r="G23">
-        <v>0.1106071423925042</v>
+        <v>0.04690813574791969</v>
       </c>
       <c r="H23">
-        <v>-4.263842215353688E-2</v>
+        <v>-0.03736746341469853</v>
       </c>
       <c r="I23">
-        <v>-1.2446777009871081E-2</v>
+        <v>-0.01244611460984458</v>
       </c>
       <c r="J23">
-        <v>-0.31723076152320218</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
+        <v>-0.3187019479903064</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C24">
-        <v>4.5387326391493052E-2</v>
+        <v>0.04483890995355639</v>
       </c>
       <c r="E24">
-        <v>0.66686448382657926</v>
+        <v>0.6668644838265793</v>
       </c>
       <c r="F24">
-        <v>-0.68608522413697692</v>
+        <v>-0.5876221398360102</v>
       </c>
       <c r="G24">
-        <v>0.6835938052311431</v>
+        <v>0.6959210190218049</v>
       </c>
       <c r="H24">
-        <v>-2.224837106593484E-2</v>
+        <v>-0.005629947489197899</v>
       </c>
       <c r="I24">
-        <v>1.2287652491506099E-2</v>
+        <v>0.01228859233154369</v>
       </c>
       <c r="J24">
-        <v>-0.54280478135074817</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>-0.5441886656332993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C25">
-        <v>2.5076996203079851E-3</v>
+        <v>0.002464859234594369</v>
       </c>
       <c r="E25">
-        <v>-1.5653802290152091E-2</v>
+        <v>-0.01565380229015209</v>
       </c>
       <c r="F25">
-        <v>1.530085873810855E-2</v>
+        <v>0.003655880603032582</v>
       </c>
       <c r="G25">
-        <v>-2.8825676066641282E-3</v>
+        <v>-0.002472211619769656</v>
       </c>
       <c r="H25">
-        <v>1.8524336420973449E-2</v>
+        <v>0.0181516475100659</v>
       </c>
       <c r="I25">
-        <v>1.9287016131480639E-2</v>
+        <v>0.01928729318749172</v>
       </c>
       <c r="J25">
-        <v>1.9197316682154599E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
+        <v>0.01679945128897563</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C26">
-        <v>2.5072778154911119E-2</v>
+        <v>0.02548867829954713</v>
       </c>
       <c r="E26">
-        <v>2.9604575168183E-2</v>
+        <v>0.029604575168183</v>
       </c>
       <c r="F26">
-        <v>-3.3749847007870391E-2</v>
+        <v>-0.02074721525888076</v>
       </c>
       <c r="G26">
-        <v>3.2960266632918747E-2</v>
+        <v>0.02467116754115437</v>
       </c>
       <c r="H26">
-        <v>1.4547607781904309E-2</v>
+        <v>0.01505233932209357</v>
       </c>
       <c r="I26">
-        <v>1.2201717512068701E-2</v>
+        <v>0.01220217975208719</v>
       </c>
       <c r="J26">
-        <v>-3.5575821583700581E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-0.03840649868140881</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C27">
-        <v>2.198764407950576E-2</v>
+        <v>0.0216441526097661</v>
       </c>
       <c r="E27">
-        <v>-2.3679409523176379E-2</v>
+        <v>-0.02367940952317638</v>
       </c>
       <c r="F27">
-        <v>3.2409845122599583E-2</v>
+        <v>0.03009971920696352</v>
       </c>
       <c r="G27">
-        <v>-3.0922039297200828E-2</v>
+        <v>-0.0281752254241294</v>
       </c>
       <c r="H27">
-        <v>-2.1430033049201321E-2</v>
+        <v>-0.02191496026859841</v>
       </c>
       <c r="I27">
-        <v>-2.2727020749080829E-2</v>
+        <v>-0.02272681780507271</v>
       </c>
       <c r="J27">
-        <v>2.565655042136018E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.02482578237397206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C28">
-        <v>-1.506210473048419E-2</v>
+        <v>-0.01509759391590375</v>
       </c>
       <c r="E28">
-        <v>-3.7490638619625538E-3</v>
+        <v>-0.003749063861962554</v>
       </c>
       <c r="F28">
-        <v>6.1511375748517748E-4</v>
+        <v>0.003287580474801443</v>
       </c>
       <c r="G28">
-        <v>1.351745773607675E-2</v>
+        <v>0.01491650923100497</v>
       </c>
       <c r="H28">
-        <v>1.4491561539662461E-2</v>
+        <v>0.01409259425970377</v>
       </c>
       <c r="I28">
-        <v>9.3571635742865419E-3</v>
+        <v>0.009357281366291253</v>
       </c>
       <c r="J28">
-        <v>6.3502518946972194E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.005794656624408714</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C29">
-        <v>1.254715518988621E-2</v>
+        <v>0.01250631611625264</v>
       </c>
       <c r="E29">
-        <v>3.853490170139607E-3</v>
+        <v>0.003853490170139607</v>
       </c>
       <c r="F29">
-        <v>4.8117433971448563E-3</v>
+        <v>0.01293373829409526</v>
       </c>
       <c r="G29">
-        <v>-2.789452166326944E-3</v>
+        <v>-0.004174761726281804</v>
       </c>
       <c r="H29">
-        <v>-8.5134197325367894E-3</v>
+        <v>-0.008002611488104459</v>
       </c>
       <c r="I29">
-        <v>-7.6448914737956572E-3</v>
+        <v>-0.00764560302582412</v>
       </c>
       <c r="J29">
-        <v>-1.276141319991414E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-0.0137836291158552</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C30">
-        <v>3.4085716243428652E-3</v>
+        <v>0.003413737576549503</v>
       </c>
       <c r="E30">
-        <v>9.3023840520953607E-4</v>
+        <v>0.0009302384052095361</v>
       </c>
       <c r="F30">
-        <v>-6.5675258239786842E-3</v>
+        <v>-0.0124115332554731</v>
       </c>
       <c r="G30">
-        <v>3.4744712622627369E-3</v>
+        <v>0.006810400281800915</v>
       </c>
       <c r="H30">
-        <v>3.192073279682931E-3</v>
+        <v>0.003147726845909073</v>
       </c>
       <c r="I30">
-        <v>2.8341837293673492E-3</v>
+        <v>0.00283437025737481</v>
       </c>
       <c r="J30">
-        <v>5.7191465245896526E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.00354139195492527</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C31">
-        <v>-3.9627021745080862E-3</v>
+        <v>-0.004047923489916939</v>
       </c>
       <c r="E31">
-        <v>9.8362603294504126E-3</v>
+        <v>0.009836260329450413</v>
       </c>
       <c r="F31">
-        <v>-8.2715652894755545E-3</v>
+        <v>-0.007857736334602971</v>
       </c>
       <c r="G31">
-        <v>1.0945694752440369E-2</v>
+        <v>0.01494529965587539</v>
       </c>
       <c r="H31">
-        <v>1.5789615799584631E-2</v>
+        <v>0.0164111325924453</v>
       </c>
       <c r="I31">
-        <v>1.6355049678201981E-2</v>
+        <v>0.01635562932622517</v>
       </c>
       <c r="J31">
-        <v>-2.8428142872015411E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-0.02654386948525206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C32">
-        <v>9.4255605050224192E-3</v>
+        <v>0.009378092631123705</v>
       </c>
       <c r="E32">
-        <v>-6.0570060022802389E-4</v>
+        <v>-0.0006057006002280239</v>
       </c>
       <c r="F32">
-        <v>-1.7820343666005471E-3</v>
+        <v>0.00143902236392284</v>
       </c>
       <c r="G32">
-        <v>4.5694257497641061E-3</v>
+        <v>0.005555258728085256</v>
       </c>
       <c r="H32">
-        <v>2.2426070337042809E-3</v>
+        <v>0.002155139318205572</v>
       </c>
       <c r="I32">
-        <v>3.2590325143612999E-3</v>
+        <v>0.003259299394371975</v>
       </c>
       <c r="J32">
-        <v>3.6337532223211029E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.003211697317246898</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C33">
-        <v>4.9563349502533974E-3</v>
+        <v>0.004859306978372279</v>
       </c>
       <c r="E33">
-        <v>-2.5922292556891701E-3</v>
+        <v>-0.00259222925568917</v>
       </c>
       <c r="F33">
-        <v>1.652195691144486E-3</v>
+        <v>-0.001651015941841666</v>
       </c>
       <c r="G33">
-        <v>-7.936204419556071E-3</v>
+        <v>-0.0052251226859695</v>
       </c>
       <c r="H33">
-        <v>-4.7179572447182891E-3</v>
+        <v>-0.004976521063060842</v>
       </c>
       <c r="I33">
-        <v>-5.3490356379614244E-3</v>
+        <v>-0.005349251061970041</v>
       </c>
       <c r="J33">
-        <v>1.5414112237651E-2</v>
+        <v>0.01505219169648533</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>